<commit_message>
Updated frame identification, changed some connectors
- `Frame Identification.pdf` now has handy arrows to the front, top left corner of each piece and an explanation of the labeling system.
- Switched hotend wiring to 20awg and connector to Micro Fit Jr.
- Fixed #42 (A/B steppers have pigtailed connectors now)
- Chasing a phantom tee nut.
</commit_message>
<xml_diff>
--- a/BOM/bill_of_materials.xlsx
+++ b/BOM/bill_of_materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\Documents\3D Print\Clockmaker\clock-3\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{C003B1B5-646F-41BC-BC6A-D207AFFCEE8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{520EAF05-FAE8-40FC-8B26-B1ACEFC0D1AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1983" uniqueCount="1055">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1980" uniqueCount="1053">
   <si>
     <t>ID</t>
   </si>
@@ -1567,6 +1567,9 @@
     <t>https://www.amazon.com/M5-0-80-Stainless-Button-Socket-Screws/dp/B077WLXQWG</t>
   </si>
   <si>
+    <t>SHCS - Stain M5.8.10</t>
+  </si>
+  <si>
     <t>PN532</t>
   </si>
   <si>
@@ -1576,6 +1579,9 @@
     <t>https://www.amazon.com/M5-0-80-Stainless-Button-Socket-Screws/dp/B078CQLGKX</t>
   </si>
   <si>
+    <t>SHCS - Stain M5.12.10</t>
+  </si>
+  <si>
     <t>200pc: https://www.amazon.com/M5-0-8-Button-Available-Stainless-Machine/dp/B07VRZYMP6</t>
   </si>
   <si>
@@ -1588,6 +1594,9 @@
     <t>https://www.amazon.com/M5-0-80-Stainless-Button-Socket-Screws/dp/B077WLQ1LZ</t>
   </si>
   <si>
+    <t>SHCS - Stain M5.16.10</t>
+  </si>
+  <si>
     <t>PN534</t>
   </si>
   <si>
@@ -1597,6 +1606,9 @@
     <t>https://www.amazon.com/M5-0-80-Stainless-Button-Socket-Screws/dp/B077WCYJB9</t>
   </si>
   <si>
+    <t>SHCS - Stain M5.25.10</t>
+  </si>
+  <si>
     <t>PN535</t>
   </si>
   <si>
@@ -1675,6 +1687,9 @@
     <t>https://www.amazon.com/20-M5-0-80-35mm-Stainless-MonsterBolts/dp/B078L3YNS3</t>
   </si>
   <si>
+    <t>â€ŽSHCS - Stain M5x16.10</t>
+  </si>
+  <si>
     <t>Door corners only. MISUMI corners ships with screws.</t>
   </si>
   <si>
@@ -3164,27 +3179,6 @@
   </si>
   <si>
     <t>For organizing parts before assembly</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/M5-0-80-Stainless-Button-Socket-Screws/dp/B077WKWHXC</t>
-  </si>
-  <si>
-    <t>‎BHCS-M-A2-M5x20.0010</t>
-  </si>
-  <si>
-    <t>‎BHCS-M-A2-M5x25.0010</t>
-  </si>
-  <si>
-    <t>‎BHCS-M-A2-M5x16.0010</t>
-  </si>
-  <si>
-    <t>‎BHCS-M-A2-M5x12.0010</t>
-  </si>
-  <si>
-    <t>‎BHCS-M-A2-M5x8.0010</t>
-  </si>
-  <si>
-    <t>SHCS - Stain M5x16.10</t>
   </si>
 </sst>
 </file>
@@ -4046,8 +4040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J292"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
-      <selection activeCell="F147" sqref="F147"/>
+    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7787,18 +7781,18 @@
         <v>471</v>
       </c>
       <c r="I146" t="s">
-        <v>1053</v>
+        <v>515</v>
       </c>
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B147" t="s">
         <v>468</v>
       </c>
       <c r="C147" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="D147" t="s">
         <v>20</v>
@@ -7810,27 +7804,27 @@
         <v>14</v>
       </c>
       <c r="G147" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="H147" t="s">
         <v>471</v>
       </c>
       <c r="I147" t="s">
-        <v>1052</v>
+        <v>519</v>
       </c>
       <c r="J147" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="B148" t="s">
         <v>468</v>
       </c>
       <c r="C148" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="D148" t="s">
         <v>20</v>
@@ -7842,24 +7836,24 @@
         <v>14</v>
       </c>
       <c r="G148" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="H148" t="s">
         <v>471</v>
       </c>
       <c r="I148" t="s">
-        <v>1051</v>
+        <v>524</v>
       </c>
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="B149" t="s">
         <v>468</v>
       </c>
       <c r="C149" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="D149" t="s">
         <v>20</v>
@@ -7871,24 +7865,24 @@
         <v>14</v>
       </c>
       <c r="G149" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="H149" t="s">
         <v>471</v>
       </c>
       <c r="I149" t="s">
-        <v>1050</v>
+        <v>528</v>
       </c>
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>525</v>
+        <v>529</v>
       </c>
       <c r="B150" t="s">
         <v>468</v>
       </c>
       <c r="C150" t="s">
-        <v>526</v>
+        <v>530</v>
       </c>
       <c r="D150" t="s">
         <v>20</v>
@@ -7900,24 +7894,24 @@
         <v>14</v>
       </c>
       <c r="G150" t="s">
-        <v>527</v>
+        <v>531</v>
       </c>
       <c r="H150" t="s">
         <v>27</v>
       </c>
       <c r="J150" t="s">
-        <v>528</v>
+        <v>532</v>
       </c>
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>529</v>
+        <v>533</v>
       </c>
       <c r="B151" t="s">
         <v>468</v>
       </c>
       <c r="C151" t="s">
-        <v>530</v>
+        <v>534</v>
       </c>
       <c r="D151" t="s">
         <v>20</v>
@@ -7925,25 +7919,16 @@
       <c r="E151">
         <v>4</v>
       </c>
-      <c r="G151" t="s">
-        <v>1048</v>
-      </c>
-      <c r="H151" t="s">
-        <v>471</v>
-      </c>
-      <c r="I151" t="s">
-        <v>1049</v>
-      </c>
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>531</v>
+        <v>535</v>
       </c>
       <c r="B152" t="s">
         <v>468</v>
       </c>
       <c r="C152" t="s">
-        <v>532</v>
+        <v>536</v>
       </c>
       <c r="D152" t="s">
         <v>20</v>
@@ -7952,18 +7937,18 @@
         <v>6</v>
       </c>
       <c r="J152" t="s">
-        <v>528</v>
+        <v>532</v>
       </c>
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>533</v>
+        <v>537</v>
       </c>
       <c r="B153" t="s">
         <v>468</v>
       </c>
       <c r="C153" t="s">
-        <v>534</v>
+        <v>538</v>
       </c>
       <c r="D153" t="s">
         <v>20</v>
@@ -7975,27 +7960,27 @@
         <v>14</v>
       </c>
       <c r="G153" t="s">
-        <v>535</v>
+        <v>539</v>
       </c>
       <c r="H153" t="s">
-        <v>536</v>
+        <v>540</v>
       </c>
       <c r="I153" t="s">
-        <v>537</v>
+        <v>541</v>
       </c>
       <c r="J153" t="s">
-        <v>538</v>
+        <v>542</v>
       </c>
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>539</v>
+        <v>543</v>
       </c>
       <c r="B154" t="s">
         <v>468</v>
       </c>
       <c r="C154" t="s">
-        <v>540</v>
+        <v>544</v>
       </c>
       <c r="D154" t="s">
         <v>20</v>
@@ -8007,24 +7992,24 @@
         <v>14</v>
       </c>
       <c r="G154" t="s">
-        <v>541</v>
+        <v>545</v>
       </c>
       <c r="H154" t="s">
-        <v>542</v>
+        <v>546</v>
       </c>
       <c r="J154" t="s">
-        <v>543</v>
+        <v>547</v>
       </c>
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>544</v>
+        <v>548</v>
       </c>
       <c r="B155" t="s">
         <v>468</v>
       </c>
       <c r="C155" t="s">
-        <v>545</v>
+        <v>549</v>
       </c>
       <c r="D155" t="s">
         <v>20</v>
@@ -8036,24 +8021,24 @@
         <v>14</v>
       </c>
       <c r="G155" t="s">
-        <v>546</v>
+        <v>550</v>
       </c>
       <c r="H155" t="s">
-        <v>536</v>
+        <v>540</v>
       </c>
       <c r="J155" t="s">
-        <v>547</v>
+        <v>551</v>
       </c>
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>548</v>
+        <v>552</v>
       </c>
       <c r="B156" t="s">
         <v>468</v>
       </c>
       <c r="C156" t="s">
-        <v>549</v>
+        <v>553</v>
       </c>
       <c r="D156" t="s">
         <v>20</v>
@@ -8065,27 +8050,27 @@
         <v>14</v>
       </c>
       <c r="G156" t="s">
-        <v>550</v>
+        <v>554</v>
       </c>
       <c r="H156" t="s">
         <v>471</v>
       </c>
       <c r="I156" t="s">
-        <v>1054</v>
+        <v>555</v>
       </c>
       <c r="J156" t="s">
-        <v>551</v>
+        <v>556</v>
       </c>
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>552</v>
+        <v>557</v>
       </c>
       <c r="B157" t="s">
         <v>468</v>
       </c>
       <c r="C157" t="s">
-        <v>553</v>
+        <v>558</v>
       </c>
       <c r="D157" t="s">
         <v>20</v>
@@ -8097,24 +8082,24 @@
         <v>14</v>
       </c>
       <c r="G157" t="s">
-        <v>554</v>
+        <v>559</v>
       </c>
       <c r="H157" t="s">
         <v>27</v>
       </c>
       <c r="J157" t="s">
-        <v>555</v>
+        <v>560</v>
       </c>
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>556</v>
+        <v>561</v>
       </c>
       <c r="B158" t="s">
         <v>468</v>
       </c>
       <c r="C158" t="s">
-        <v>540</v>
+        <v>544</v>
       </c>
       <c r="D158" t="s">
         <v>20</v>
@@ -8126,18 +8111,18 @@
         <v>27</v>
       </c>
       <c r="J158" t="s">
-        <v>557</v>
+        <v>562</v>
       </c>
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>558</v>
+        <v>563</v>
       </c>
       <c r="B159" t="s">
         <v>468</v>
       </c>
       <c r="C159" t="s">
-        <v>559</v>
+        <v>564</v>
       </c>
       <c r="D159" t="s">
         <v>20</v>
@@ -8149,18 +8134,18 @@
         <v>27</v>
       </c>
       <c r="J159" t="s">
-        <v>560</v>
+        <v>565</v>
       </c>
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>561</v>
+        <v>566</v>
       </c>
       <c r="B160" t="s">
         <v>468</v>
       </c>
       <c r="C160" t="s">
-        <v>562</v>
+        <v>567</v>
       </c>
       <c r="D160" t="s">
         <v>20</v>
@@ -8172,24 +8157,24 @@
         <v>36</v>
       </c>
       <c r="G160" t="s">
-        <v>563</v>
+        <v>568</v>
       </c>
       <c r="H160" t="s">
         <v>27</v>
       </c>
       <c r="J160" t="s">
-        <v>564</v>
+        <v>569</v>
       </c>
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>565</v>
+        <v>570</v>
       </c>
       <c r="B161" t="s">
         <v>468</v>
       </c>
       <c r="C161" t="s">
-        <v>566</v>
+        <v>571</v>
       </c>
       <c r="D161" t="s">
         <v>20</v>
@@ -8201,7 +8186,7 @@
         <v>14</v>
       </c>
       <c r="G161" t="s">
-        <v>567</v>
+        <v>572</v>
       </c>
       <c r="H161" t="s">
         <v>27</v>
@@ -8209,13 +8194,13 @@
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>568</v>
+        <v>573</v>
       </c>
       <c r="B162" t="s">
         <v>468</v>
       </c>
       <c r="C162" t="s">
-        <v>569</v>
+        <v>574</v>
       </c>
       <c r="D162" t="s">
         <v>20</v>
@@ -8227,7 +8212,7 @@
         <v>14</v>
       </c>
       <c r="G162" t="s">
-        <v>567</v>
+        <v>572</v>
       </c>
       <c r="H162" t="s">
         <v>27</v>
@@ -8235,13 +8220,13 @@
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>570</v>
+        <v>575</v>
       </c>
       <c r="B163" t="s">
         <v>468</v>
       </c>
       <c r="C163" t="s">
-        <v>571</v>
+        <v>576</v>
       </c>
       <c r="D163" t="s">
         <v>20</v>
@@ -8253,7 +8238,7 @@
         <v>14</v>
       </c>
       <c r="G163" t="s">
-        <v>567</v>
+        <v>572</v>
       </c>
       <c r="H163" t="s">
         <v>27</v>
@@ -8261,13 +8246,13 @@
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>572</v>
+        <v>577</v>
       </c>
       <c r="B164" t="s">
         <v>468</v>
       </c>
       <c r="C164" t="s">
-        <v>573</v>
+        <v>578</v>
       </c>
       <c r="D164" t="s">
         <v>20</v>
@@ -8279,7 +8264,7 @@
         <v>14</v>
       </c>
       <c r="G164" t="s">
-        <v>574</v>
+        <v>579</v>
       </c>
       <c r="H164" t="s">
         <v>27</v>
@@ -8287,13 +8272,13 @@
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>575</v>
+        <v>580</v>
       </c>
       <c r="B165" t="s">
         <v>468</v>
       </c>
       <c r="C165" t="s">
-        <v>576</v>
+        <v>581</v>
       </c>
       <c r="D165" t="s">
         <v>20</v>
@@ -8305,7 +8290,7 @@
         <v>14</v>
       </c>
       <c r="G165" t="s">
-        <v>574</v>
+        <v>579</v>
       </c>
       <c r="H165" t="s">
         <v>27</v>
@@ -8313,13 +8298,13 @@
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>577</v>
+        <v>582</v>
       </c>
       <c r="B166" t="s">
         <v>468</v>
       </c>
       <c r="C166" t="s">
-        <v>578</v>
+        <v>583</v>
       </c>
       <c r="D166" t="s">
         <v>20</v>
@@ -8331,7 +8316,7 @@
         <v>14</v>
       </c>
       <c r="G166" t="s">
-        <v>579</v>
+        <v>584</v>
       </c>
       <c r="H166" t="s">
         <v>27</v>
@@ -8339,13 +8324,13 @@
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>580</v>
+        <v>585</v>
       </c>
       <c r="B167" t="s">
         <v>468</v>
       </c>
       <c r="C167" t="s">
-        <v>581</v>
+        <v>586</v>
       </c>
       <c r="D167" t="s">
         <v>20</v>
@@ -8357,7 +8342,7 @@
         <v>14</v>
       </c>
       <c r="G167" t="s">
-        <v>582</v>
+        <v>587</v>
       </c>
       <c r="H167" t="s">
         <v>27</v>
@@ -8365,13 +8350,13 @@
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>583</v>
+        <v>588</v>
       </c>
       <c r="B168" t="s">
         <v>468</v>
       </c>
       <c r="C168" t="s">
-        <v>584</v>
+        <v>589</v>
       </c>
       <c r="D168" t="s">
         <v>20</v>
@@ -8383,7 +8368,7 @@
         <v>14</v>
       </c>
       <c r="G168" t="s">
-        <v>585</v>
+        <v>590</v>
       </c>
       <c r="H168" t="s">
         <v>27</v>
@@ -8391,13 +8376,13 @@
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>586</v>
+        <v>591</v>
       </c>
       <c r="B169" t="s">
         <v>468</v>
       </c>
       <c r="C169" t="s">
-        <v>587</v>
+        <v>592</v>
       </c>
       <c r="D169" t="s">
         <v>20</v>
@@ -8409,7 +8394,7 @@
         <v>14</v>
       </c>
       <c r="G169" t="s">
-        <v>588</v>
+        <v>593</v>
       </c>
       <c r="H169" t="s">
         <v>27</v>
@@ -8417,13 +8402,13 @@
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>589</v>
+        <v>594</v>
       </c>
       <c r="B170" t="s">
         <v>468</v>
       </c>
       <c r="C170" t="s">
-        <v>590</v>
+        <v>595</v>
       </c>
       <c r="D170" t="s">
         <v>20</v>
@@ -8435,24 +8420,24 @@
         <v>14</v>
       </c>
       <c r="G170" t="s">
-        <v>591</v>
+        <v>596</v>
       </c>
       <c r="H170" t="s">
         <v>27</v>
       </c>
       <c r="J170" t="s">
-        <v>592</v>
+        <v>597</v>
       </c>
     </row>
     <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>593</v>
+        <v>598</v>
       </c>
       <c r="B171" t="s">
         <v>468</v>
       </c>
       <c r="C171" t="s">
-        <v>594</v>
+        <v>599</v>
       </c>
       <c r="D171" t="s">
         <v>20</v>
@@ -8464,24 +8449,24 @@
         <v>14</v>
       </c>
       <c r="G171" t="s">
-        <v>595</v>
+        <v>600</v>
       </c>
       <c r="H171" t="s">
         <v>27</v>
       </c>
       <c r="J171" t="s">
-        <v>596</v>
+        <v>601</v>
       </c>
     </row>
     <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>597</v>
+        <v>602</v>
       </c>
       <c r="B172" t="s">
         <v>468</v>
       </c>
       <c r="C172" t="s">
-        <v>598</v>
+        <v>603</v>
       </c>
       <c r="D172" t="s">
         <v>20</v>
@@ -8493,24 +8478,24 @@
         <v>14</v>
       </c>
       <c r="G172" t="s">
-        <v>546</v>
+        <v>550</v>
       </c>
       <c r="H172" t="s">
-        <v>536</v>
+        <v>540</v>
       </c>
       <c r="J172" t="s">
-        <v>599</v>
+        <v>604</v>
       </c>
     </row>
     <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>600</v>
+        <v>605</v>
       </c>
       <c r="B173" t="s">
         <v>468</v>
       </c>
       <c r="C173" t="s">
-        <v>601</v>
+        <v>606</v>
       </c>
       <c r="D173" t="s">
         <v>20</v>
@@ -8522,21 +8507,21 @@
         <v>14</v>
       </c>
       <c r="G173" t="s">
-        <v>602</v>
+        <v>607</v>
       </c>
       <c r="H173" t="s">
-        <v>536</v>
+        <v>540</v>
       </c>
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>603</v>
+        <v>608</v>
       </c>
       <c r="B174" t="s">
         <v>468</v>
       </c>
       <c r="C174" t="s">
-        <v>604</v>
+        <v>609</v>
       </c>
       <c r="D174" t="s">
         <v>20</v>
@@ -8548,21 +8533,21 @@
         <v>14</v>
       </c>
       <c r="G174" t="s">
-        <v>605</v>
+        <v>610</v>
       </c>
       <c r="H174" t="s">
-        <v>606</v>
+        <v>611</v>
       </c>
     </row>
     <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>607</v>
+        <v>612</v>
       </c>
       <c r="B175" t="s">
-        <v>608</v>
+        <v>613</v>
       </c>
       <c r="C175" t="s">
-        <v>609</v>
+        <v>614</v>
       </c>
       <c r="D175" t="s">
         <v>20</v>
@@ -8574,24 +8559,24 @@
         <v>14</v>
       </c>
       <c r="G175" t="s">
-        <v>610</v>
+        <v>615</v>
       </c>
       <c r="H175" t="s">
-        <v>611</v>
+        <v>616</v>
       </c>
       <c r="I175" t="s">
-        <v>612</v>
+        <v>617</v>
       </c>
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
+        <v>618</v>
+      </c>
+      <c r="B176" t="s">
         <v>613</v>
       </c>
-      <c r="B176" t="s">
-        <v>608</v>
-      </c>
       <c r="C176" t="s">
-        <v>614</v>
+        <v>619</v>
       </c>
       <c r="D176" t="s">
         <v>20</v>
@@ -8603,24 +8588,24 @@
         <v>14</v>
       </c>
       <c r="G176" t="s">
-        <v>615</v>
+        <v>620</v>
       </c>
       <c r="H176" t="s">
-        <v>611</v>
+        <v>616</v>
       </c>
       <c r="I176" t="s">
-        <v>616</v>
+        <v>621</v>
       </c>
     </row>
     <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>617</v>
+        <v>622</v>
       </c>
       <c r="B177" t="s">
-        <v>608</v>
+        <v>613</v>
       </c>
       <c r="C177" t="s">
-        <v>618</v>
+        <v>623</v>
       </c>
       <c r="D177" t="s">
         <v>20</v>
@@ -8632,24 +8617,24 @@
         <v>14</v>
       </c>
       <c r="G177" t="s">
-        <v>619</v>
+        <v>624</v>
       </c>
       <c r="H177" t="s">
-        <v>620</v>
+        <v>625</v>
       </c>
       <c r="I177" t="s">
-        <v>621</v>
+        <v>626</v>
       </c>
     </row>
     <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>622</v>
+        <v>627</v>
       </c>
       <c r="B178" t="s">
-        <v>608</v>
+        <v>613</v>
       </c>
       <c r="C178" t="s">
-        <v>623</v>
+        <v>628</v>
       </c>
       <c r="D178" t="s">
         <v>20</v>
@@ -8661,7 +8646,7 @@
         <v>14</v>
       </c>
       <c r="G178" t="s">
-        <v>624</v>
+        <v>629</v>
       </c>
       <c r="H178" t="s">
         <v>27</v>
@@ -8669,13 +8654,13 @@
     </row>
     <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>625</v>
+        <v>630</v>
       </c>
       <c r="B179" t="s">
-        <v>608</v>
+        <v>613</v>
       </c>
       <c r="C179" t="s">
-        <v>626</v>
+        <v>631</v>
       </c>
       <c r="D179" t="s">
         <v>49</v>
@@ -8687,24 +8672,24 @@
         <v>14</v>
       </c>
       <c r="G179" t="s">
-        <v>627</v>
+        <v>632</v>
       </c>
       <c r="H179" t="s">
-        <v>628</v>
+        <v>633</v>
       </c>
       <c r="I179" t="s">
-        <v>629</v>
+        <v>634</v>
       </c>
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>630</v>
+        <v>635</v>
       </c>
       <c r="B180" t="s">
-        <v>608</v>
+        <v>613</v>
       </c>
       <c r="C180" t="s">
-        <v>631</v>
+        <v>636</v>
       </c>
       <c r="D180" t="s">
         <v>20</v>
@@ -8716,24 +8701,24 @@
         <v>14</v>
       </c>
       <c r="G180" t="s">
-        <v>632</v>
+        <v>637</v>
       </c>
       <c r="H180" t="s">
-        <v>611</v>
+        <v>616</v>
       </c>
       <c r="I180" t="s">
-        <v>633</v>
+        <v>638</v>
       </c>
     </row>
     <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>634</v>
+        <v>639</v>
       </c>
       <c r="B181" t="s">
-        <v>608</v>
+        <v>613</v>
       </c>
       <c r="C181" t="s">
-        <v>635</v>
+        <v>640</v>
       </c>
       <c r="D181" t="s">
         <v>20</v>
@@ -8745,24 +8730,24 @@
         <v>14</v>
       </c>
       <c r="G181" t="s">
-        <v>636</v>
+        <v>641</v>
       </c>
       <c r="H181" t="s">
-        <v>637</v>
+        <v>642</v>
       </c>
       <c r="I181" t="s">
-        <v>638</v>
+        <v>643</v>
       </c>
     </row>
     <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>639</v>
+        <v>644</v>
       </c>
       <c r="B182" t="s">
-        <v>608</v>
+        <v>613</v>
       </c>
       <c r="C182" t="s">
-        <v>640</v>
+        <v>645</v>
       </c>
       <c r="D182" t="s">
         <v>20</v>
@@ -8774,24 +8759,24 @@
         <v>14</v>
       </c>
       <c r="G182" t="s">
-        <v>641</v>
+        <v>646</v>
       </c>
       <c r="H182" t="s">
-        <v>642</v>
+        <v>647</v>
       </c>
       <c r="I182" t="s">
-        <v>643</v>
+        <v>648</v>
       </c>
     </row>
     <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>644</v>
+        <v>649</v>
       </c>
       <c r="B183" t="s">
-        <v>608</v>
+        <v>613</v>
       </c>
       <c r="C183" t="s">
-        <v>645</v>
+        <v>650</v>
       </c>
       <c r="D183" t="s">
         <v>20</v>
@@ -8803,24 +8788,24 @@
         <v>14</v>
       </c>
       <c r="G183" t="s">
-        <v>641</v>
+        <v>646</v>
       </c>
       <c r="H183" t="s">
-        <v>642</v>
+        <v>647</v>
       </c>
       <c r="I183" t="s">
-        <v>643</v>
+        <v>648</v>
       </c>
     </row>
     <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>646</v>
+        <v>651</v>
       </c>
       <c r="B184" t="s">
-        <v>608</v>
+        <v>613</v>
       </c>
       <c r="C184" t="s">
-        <v>647</v>
+        <v>652</v>
       </c>
       <c r="D184" t="s">
         <v>20</v>
@@ -8832,24 +8817,24 @@
         <v>14</v>
       </c>
       <c r="G184" t="s">
-        <v>648</v>
+        <v>653</v>
       </c>
       <c r="H184" t="s">
-        <v>637</v>
+        <v>642</v>
       </c>
       <c r="I184" t="s">
-        <v>649</v>
+        <v>654</v>
       </c>
     </row>
     <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>650</v>
+        <v>655</v>
       </c>
       <c r="B185" t="s">
-        <v>608</v>
+        <v>613</v>
       </c>
       <c r="C185" t="s">
-        <v>651</v>
+        <v>656</v>
       </c>
       <c r="D185" t="s">
         <v>20</v>
@@ -8861,24 +8846,24 @@
         <v>14</v>
       </c>
       <c r="G185" t="s">
-        <v>652</v>
+        <v>657</v>
       </c>
       <c r="H185" t="s">
-        <v>637</v>
+        <v>642</v>
       </c>
       <c r="I185" t="s">
-        <v>653</v>
+        <v>658</v>
       </c>
     </row>
     <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>654</v>
+        <v>659</v>
       </c>
       <c r="B186" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C186" t="s">
-        <v>656</v>
+        <v>661</v>
       </c>
       <c r="D186" t="s">
         <v>20</v>
@@ -8890,24 +8875,24 @@
         <v>112</v>
       </c>
       <c r="G186" t="s">
-        <v>657</v>
+        <v>662</v>
       </c>
       <c r="H186" t="s">
         <v>508</v>
       </c>
       <c r="I186" t="s">
-        <v>658</v>
+        <v>663</v>
       </c>
     </row>
     <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>659</v>
+        <v>664</v>
       </c>
       <c r="B187" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C187" t="s">
-        <v>660</v>
+        <v>665</v>
       </c>
       <c r="D187" t="s">
         <v>20</v>
@@ -8919,21 +8904,21 @@
         <v>14</v>
       </c>
       <c r="G187" t="s">
-        <v>661</v>
+        <v>666</v>
       </c>
       <c r="H187" t="s">
-        <v>542</v>
+        <v>546</v>
       </c>
     </row>
     <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>662</v>
+        <v>667</v>
       </c>
       <c r="B188" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C188" t="s">
-        <v>663</v>
+        <v>668</v>
       </c>
       <c r="D188" t="s">
         <v>20</v>
@@ -8945,24 +8930,24 @@
         <v>112</v>
       </c>
       <c r="G188" t="s">
-        <v>664</v>
+        <v>669</v>
       </c>
       <c r="H188" t="s">
         <v>508</v>
       </c>
       <c r="I188" t="s">
-        <v>665</v>
+        <v>670</v>
       </c>
     </row>
     <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>666</v>
+        <v>671</v>
       </c>
       <c r="B189" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C189" t="s">
-        <v>667</v>
+        <v>672</v>
       </c>
       <c r="D189" t="s">
         <v>20</v>
@@ -8974,24 +8959,24 @@
         <v>112</v>
       </c>
       <c r="G189" t="s">
-        <v>668</v>
+        <v>673</v>
       </c>
       <c r="H189" t="s">
         <v>508</v>
       </c>
       <c r="I189" t="s">
-        <v>669</v>
+        <v>674</v>
       </c>
     </row>
     <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>670</v>
+        <v>675</v>
       </c>
       <c r="B190" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C190" t="s">
-        <v>671</v>
+        <v>676</v>
       </c>
       <c r="D190" t="s">
         <v>20</v>
@@ -9003,24 +8988,24 @@
         <v>112</v>
       </c>
       <c r="G190" t="s">
-        <v>672</v>
+        <v>677</v>
       </c>
       <c r="H190" t="s">
         <v>508</v>
       </c>
       <c r="I190" t="s">
-        <v>673</v>
+        <v>678</v>
       </c>
     </row>
     <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>674</v>
+        <v>679</v>
       </c>
       <c r="B191" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C191" t="s">
-        <v>675</v>
+        <v>680</v>
       </c>
       <c r="D191" t="s">
         <v>20</v>
@@ -9032,27 +9017,27 @@
         <v>112</v>
       </c>
       <c r="G191" t="s">
-        <v>676</v>
+        <v>681</v>
       </c>
       <c r="H191" t="s">
         <v>508</v>
       </c>
       <c r="I191" t="s">
-        <v>677</v>
+        <v>682</v>
       </c>
       <c r="J191" t="s">
-        <v>678</v>
+        <v>683</v>
       </c>
     </row>
     <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>679</v>
+        <v>684</v>
       </c>
       <c r="B192" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C192" t="s">
-        <v>680</v>
+        <v>685</v>
       </c>
       <c r="D192" t="s">
         <v>20</v>
@@ -9064,27 +9049,27 @@
         <v>112</v>
       </c>
       <c r="G192" t="s">
-        <v>676</v>
+        <v>681</v>
       </c>
       <c r="H192" t="s">
         <v>508</v>
       </c>
       <c r="I192" t="s">
-        <v>677</v>
+        <v>682</v>
       </c>
       <c r="J192" t="s">
-        <v>678</v>
+        <v>683</v>
       </c>
     </row>
     <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>681</v>
+        <v>686</v>
       </c>
       <c r="B193" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C193" t="s">
-        <v>682</v>
+        <v>687</v>
       </c>
       <c r="D193" t="s">
         <v>20</v>
@@ -9096,24 +9081,24 @@
         <v>14</v>
       </c>
       <c r="G193" t="s">
-        <v>683</v>
+        <v>688</v>
       </c>
       <c r="H193" t="s">
         <v>27</v>
       </c>
       <c r="J193" t="s">
-        <v>684</v>
+        <v>689</v>
       </c>
     </row>
     <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>685</v>
+        <v>690</v>
       </c>
       <c r="B194" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C194" t="s">
-        <v>686</v>
+        <v>691</v>
       </c>
       <c r="D194" t="s">
         <v>20</v>
@@ -9125,27 +9110,27 @@
         <v>112</v>
       </c>
       <c r="G194" t="s">
-        <v>687</v>
+        <v>692</v>
       </c>
       <c r="H194" t="s">
         <v>508</v>
       </c>
       <c r="I194" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
       <c r="J194" t="s">
-        <v>689</v>
+        <v>694</v>
       </c>
     </row>
     <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>690</v>
+        <v>695</v>
       </c>
       <c r="B195" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C195" t="s">
-        <v>691</v>
+        <v>696</v>
       </c>
       <c r="D195" t="s">
         <v>20</v>
@@ -9157,27 +9142,27 @@
         <v>112</v>
       </c>
       <c r="G195" t="s">
-        <v>692</v>
+        <v>697</v>
       </c>
       <c r="H195" t="s">
         <v>508</v>
       </c>
       <c r="I195" t="s">
-        <v>693</v>
+        <v>698</v>
       </c>
       <c r="J195" t="s">
-        <v>694</v>
+        <v>699</v>
       </c>
     </row>
     <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>695</v>
+        <v>700</v>
       </c>
       <c r="B196" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C196" t="s">
-        <v>696</v>
+        <v>701</v>
       </c>
       <c r="D196" t="s">
         <v>20</v>
@@ -9189,27 +9174,27 @@
         <v>112</v>
       </c>
       <c r="G196" t="s">
-        <v>697</v>
+        <v>702</v>
       </c>
       <c r="H196" t="s">
         <v>508</v>
       </c>
       <c r="I196" t="s">
-        <v>698</v>
+        <v>703</v>
       </c>
       <c r="J196" t="s">
-        <v>699</v>
+        <v>704</v>
       </c>
     </row>
     <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>700</v>
+        <v>705</v>
       </c>
       <c r="B197" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C197" t="s">
-        <v>701</v>
+        <v>706</v>
       </c>
       <c r="D197" t="s">
         <v>20</v>
@@ -9221,27 +9206,27 @@
         <v>112</v>
       </c>
       <c r="G197" t="s">
-        <v>702</v>
+        <v>707</v>
       </c>
       <c r="H197" t="s">
         <v>508</v>
       </c>
       <c r="I197" t="s">
-        <v>703</v>
+        <v>708</v>
       </c>
       <c r="J197" t="s">
-        <v>704</v>
+        <v>709</v>
       </c>
     </row>
     <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>705</v>
+        <v>710</v>
       </c>
       <c r="B198" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C198" t="s">
-        <v>706</v>
+        <v>711</v>
       </c>
       <c r="D198" t="s">
         <v>20</v>
@@ -9253,27 +9238,27 @@
         <v>112</v>
       </c>
       <c r="G198" t="s">
-        <v>707</v>
+        <v>712</v>
       </c>
       <c r="H198" t="s">
         <v>508</v>
       </c>
       <c r="I198" t="s">
-        <v>708</v>
+        <v>713</v>
       </c>
       <c r="J198" t="s">
-        <v>709</v>
+        <v>714</v>
       </c>
     </row>
     <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>710</v>
+        <v>715</v>
       </c>
       <c r="B199" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C199" t="s">
-        <v>711</v>
+        <v>716</v>
       </c>
       <c r="D199" t="s">
         <v>20</v>
@@ -9285,27 +9270,27 @@
         <v>112</v>
       </c>
       <c r="G199" t="s">
-        <v>712</v>
+        <v>717</v>
       </c>
       <c r="H199" t="s">
         <v>508</v>
       </c>
       <c r="I199" t="s">
-        <v>713</v>
+        <v>718</v>
       </c>
       <c r="J199" t="s">
-        <v>714</v>
+        <v>719</v>
       </c>
     </row>
     <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>715</v>
+        <v>720</v>
       </c>
       <c r="B200" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C200" t="s">
-        <v>716</v>
+        <v>721</v>
       </c>
       <c r="D200" t="s">
         <v>20</v>
@@ -9317,27 +9302,27 @@
         <v>112</v>
       </c>
       <c r="G200" t="s">
-        <v>717</v>
+        <v>722</v>
       </c>
       <c r="H200" t="s">
         <v>508</v>
       </c>
       <c r="I200" t="s">
-        <v>718</v>
+        <v>723</v>
       </c>
       <c r="J200" t="s">
-        <v>719</v>
+        <v>724</v>
       </c>
     </row>
     <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>720</v>
+        <v>725</v>
       </c>
       <c r="B201" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C201" t="s">
-        <v>721</v>
+        <v>726</v>
       </c>
       <c r="D201" t="s">
         <v>20</v>
@@ -9349,27 +9334,27 @@
         <v>112</v>
       </c>
       <c r="G201" t="s">
-        <v>722</v>
+        <v>727</v>
       </c>
       <c r="H201" t="s">
         <v>508</v>
       </c>
       <c r="I201" t="s">
-        <v>723</v>
+        <v>728</v>
       </c>
       <c r="J201" t="s">
-        <v>719</v>
+        <v>724</v>
       </c>
     </row>
     <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>724</v>
+        <v>729</v>
       </c>
       <c r="B202" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C202" t="s">
-        <v>725</v>
+        <v>730</v>
       </c>
       <c r="D202" t="s">
         <v>20</v>
@@ -9381,27 +9366,27 @@
         <v>112</v>
       </c>
       <c r="G202" t="s">
-        <v>726</v>
+        <v>731</v>
       </c>
       <c r="H202" t="s">
         <v>508</v>
       </c>
       <c r="I202" t="s">
-        <v>727</v>
+        <v>732</v>
       </c>
       <c r="J202" t="s">
-        <v>728</v>
+        <v>733</v>
       </c>
     </row>
     <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>729</v>
+        <v>734</v>
       </c>
       <c r="B203" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C203" t="s">
-        <v>730</v>
+        <v>735</v>
       </c>
       <c r="D203" t="s">
         <v>20</v>
@@ -9413,27 +9398,27 @@
         <v>112</v>
       </c>
       <c r="G203" t="s">
-        <v>731</v>
+        <v>736</v>
       </c>
       <c r="H203" t="s">
         <v>508</v>
       </c>
       <c r="I203" t="s">
-        <v>732</v>
+        <v>737</v>
       </c>
       <c r="J203" t="s">
-        <v>733</v>
+        <v>738</v>
       </c>
     </row>
     <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>734</v>
+        <v>739</v>
       </c>
       <c r="B204" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C204" t="s">
-        <v>735</v>
+        <v>740</v>
       </c>
       <c r="D204" t="s">
         <v>20</v>
@@ -9445,27 +9430,27 @@
         <v>112</v>
       </c>
       <c r="G204" t="s">
-        <v>736</v>
+        <v>741</v>
       </c>
       <c r="H204" t="s">
         <v>508</v>
       </c>
       <c r="I204" t="s">
-        <v>737</v>
+        <v>742</v>
       </c>
       <c r="J204" t="s">
-        <v>738</v>
+        <v>743</v>
       </c>
     </row>
     <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>739</v>
+        <v>744</v>
       </c>
       <c r="B205" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C205" t="s">
-        <v>740</v>
+        <v>745</v>
       </c>
       <c r="D205" t="s">
         <v>20</v>
@@ -9477,27 +9462,27 @@
         <v>112</v>
       </c>
       <c r="G205" t="s">
-        <v>741</v>
+        <v>746</v>
       </c>
       <c r="H205" t="s">
         <v>508</v>
       </c>
       <c r="I205" t="s">
-        <v>742</v>
+        <v>747</v>
       </c>
       <c r="J205" t="s">
-        <v>743</v>
+        <v>748</v>
       </c>
     </row>
     <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>744</v>
+        <v>749</v>
       </c>
       <c r="B206" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C206" t="s">
-        <v>745</v>
+        <v>750</v>
       </c>
       <c r="D206" t="s">
         <v>20</v>
@@ -9509,27 +9494,27 @@
         <v>112</v>
       </c>
       <c r="G206" t="s">
-        <v>746</v>
+        <v>751</v>
       </c>
       <c r="H206" t="s">
         <v>508</v>
       </c>
       <c r="I206" t="s">
-        <v>747</v>
+        <v>752</v>
       </c>
       <c r="J206" t="s">
-        <v>748</v>
+        <v>753</v>
       </c>
     </row>
     <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>749</v>
+        <v>754</v>
       </c>
       <c r="B207" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C207" t="s">
-        <v>750</v>
+        <v>755</v>
       </c>
       <c r="D207" t="s">
         <v>20</v>
@@ -9541,27 +9526,27 @@
         <v>112</v>
       </c>
       <c r="G207" t="s">
-        <v>751</v>
+        <v>756</v>
       </c>
       <c r="H207" t="s">
         <v>508</v>
       </c>
       <c r="I207" t="s">
-        <v>752</v>
+        <v>757</v>
       </c>
       <c r="J207" t="s">
-        <v>753</v>
+        <v>758</v>
       </c>
     </row>
     <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>754</v>
+        <v>759</v>
       </c>
       <c r="B208" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C208" t="s">
-        <v>755</v>
+        <v>760</v>
       </c>
       <c r="D208" t="s">
         <v>20</v>
@@ -9576,18 +9561,18 @@
         <v>26</v>
       </c>
       <c r="J208" t="s">
-        <v>756</v>
+        <v>761</v>
       </c>
     </row>
     <row r="209" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>757</v>
+        <v>762</v>
       </c>
       <c r="B209" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C209" t="s">
-        <v>758</v>
+        <v>763</v>
       </c>
       <c r="D209" t="s">
         <v>20</v>
@@ -9602,18 +9587,18 @@
         <v>26</v>
       </c>
       <c r="J209" t="s">
-        <v>759</v>
+        <v>764</v>
       </c>
     </row>
     <row r="210" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>760</v>
+        <v>765</v>
       </c>
       <c r="B210" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C210" t="s">
-        <v>761</v>
+        <v>766</v>
       </c>
       <c r="D210" t="s">
         <v>20</v>
@@ -9630,13 +9615,13 @@
     </row>
     <row r="211" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>762</v>
+        <v>767</v>
       </c>
       <c r="B211" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C211" t="s">
-        <v>763</v>
+        <v>768</v>
       </c>
       <c r="D211" t="s">
         <v>20</v>
@@ -9653,13 +9638,13 @@
     </row>
     <row r="212" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>764</v>
+        <v>769</v>
       </c>
       <c r="B212" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C212" t="s">
-        <v>765</v>
+        <v>770</v>
       </c>
       <c r="D212" t="s">
         <v>20</v>
@@ -9676,13 +9661,13 @@
     </row>
     <row r="213" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>766</v>
+        <v>771</v>
       </c>
       <c r="B213" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C213" t="s">
-        <v>767</v>
+        <v>772</v>
       </c>
       <c r="D213" t="s">
         <v>20</v>
@@ -9699,13 +9684,13 @@
     </row>
     <row r="214" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>768</v>
+        <v>773</v>
       </c>
       <c r="B214" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C214" t="s">
-        <v>769</v>
+        <v>774</v>
       </c>
       <c r="D214" t="s">
         <v>20</v>
@@ -9722,13 +9707,13 @@
     </row>
     <row r="215" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>770</v>
+        <v>775</v>
       </c>
       <c r="B215" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C215" t="s">
-        <v>771</v>
+        <v>776</v>
       </c>
       <c r="D215" t="s">
         <v>20</v>
@@ -9745,13 +9730,13 @@
     </row>
     <row r="216" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>772</v>
+        <v>777</v>
       </c>
       <c r="B216" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C216" t="s">
-        <v>773</v>
+        <v>778</v>
       </c>
       <c r="D216" t="s">
         <v>20</v>
@@ -9768,13 +9753,13 @@
     </row>
     <row r="217" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>774</v>
+        <v>779</v>
       </c>
       <c r="B217" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C217" t="s">
-        <v>775</v>
+        <v>780</v>
       </c>
       <c r="D217" t="s">
         <v>20</v>
@@ -9791,13 +9776,13 @@
     </row>
     <row r="218" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>776</v>
+        <v>781</v>
       </c>
       <c r="B218" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C218" t="s">
-        <v>777</v>
+        <v>782</v>
       </c>
       <c r="D218" t="s">
         <v>20</v>
@@ -9814,13 +9799,13 @@
     </row>
     <row r="219" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>778</v>
+        <v>783</v>
       </c>
       <c r="B219" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C219" t="s">
-        <v>779</v>
+        <v>784</v>
       </c>
       <c r="D219" t="s">
         <v>20</v>
@@ -9837,13 +9822,13 @@
     </row>
     <row r="220" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>780</v>
+        <v>785</v>
       </c>
       <c r="B220" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C220" t="s">
-        <v>781</v>
+        <v>786</v>
       </c>
       <c r="D220" t="s">
         <v>20</v>
@@ -9860,13 +9845,13 @@
     </row>
     <row r="221" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>782</v>
+        <v>787</v>
       </c>
       <c r="B221" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C221" t="s">
-        <v>783</v>
+        <v>788</v>
       </c>
       <c r="D221" t="s">
         <v>20</v>
@@ -9883,13 +9868,13 @@
     </row>
     <row r="222" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>784</v>
+        <v>789</v>
       </c>
       <c r="B222" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C222" t="s">
-        <v>785</v>
+        <v>790</v>
       </c>
       <c r="D222" t="s">
         <v>20</v>
@@ -9904,18 +9889,18 @@
         <v>26</v>
       </c>
       <c r="J222" t="s">
-        <v>786</v>
+        <v>791</v>
       </c>
     </row>
     <row r="223" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>787</v>
+        <v>792</v>
       </c>
       <c r="B223" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C223" t="s">
-        <v>788</v>
+        <v>793</v>
       </c>
       <c r="D223" t="s">
         <v>20</v>
@@ -9924,18 +9909,18 @@
         <v>1</v>
       </c>
       <c r="J223" t="s">
-        <v>789</v>
+        <v>794</v>
       </c>
     </row>
     <row r="224" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>790</v>
+        <v>795</v>
       </c>
       <c r="B224" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C224" t="s">
-        <v>791</v>
+        <v>796</v>
       </c>
       <c r="D224" t="s">
         <v>20</v>
@@ -9944,18 +9929,18 @@
         <v>1</v>
       </c>
       <c r="J224" t="s">
-        <v>789</v>
+        <v>794</v>
       </c>
     </row>
     <row r="225" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>792</v>
+        <v>797</v>
       </c>
       <c r="B225" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C225" t="s">
-        <v>793</v>
+        <v>798</v>
       </c>
       <c r="D225" t="s">
         <v>20</v>
@@ -9964,18 +9949,18 @@
         <v>1</v>
       </c>
       <c r="J225" t="s">
-        <v>789</v>
+        <v>794</v>
       </c>
     </row>
     <row r="226" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>794</v>
+        <v>799</v>
       </c>
       <c r="B226" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C226" t="s">
-        <v>795</v>
+        <v>800</v>
       </c>
       <c r="D226" t="s">
         <v>20</v>
@@ -9984,18 +9969,18 @@
         <v>1</v>
       </c>
       <c r="J226" t="s">
-        <v>796</v>
+        <v>801</v>
       </c>
     </row>
     <row r="227" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>797</v>
+        <v>802</v>
       </c>
       <c r="B227" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C227" t="s">
-        <v>798</v>
+        <v>803</v>
       </c>
       <c r="D227" t="s">
         <v>20</v>
@@ -10004,18 +9989,18 @@
         <v>1</v>
       </c>
       <c r="J227" t="s">
-        <v>796</v>
+        <v>801</v>
       </c>
     </row>
     <row r="228" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>799</v>
+        <v>804</v>
       </c>
       <c r="B228" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C228" t="s">
-        <v>800</v>
+        <v>805</v>
       </c>
       <c r="D228" t="s">
         <v>20</v>
@@ -10024,18 +10009,18 @@
         <v>1</v>
       </c>
       <c r="J228" t="s">
-        <v>796</v>
+        <v>801</v>
       </c>
     </row>
     <row r="229" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>801</v>
+        <v>806</v>
       </c>
       <c r="B229" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C229" t="s">
-        <v>802</v>
+        <v>807</v>
       </c>
       <c r="D229" t="s">
         <v>20</v>
@@ -10044,18 +10029,18 @@
         <v>1</v>
       </c>
       <c r="J229" t="s">
-        <v>803</v>
+        <v>808</v>
       </c>
     </row>
     <row r="230" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>804</v>
+        <v>809</v>
       </c>
       <c r="B230" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C230" t="s">
-        <v>805</v>
+        <v>810</v>
       </c>
       <c r="D230" t="s">
         <v>20</v>
@@ -10064,18 +10049,18 @@
         <v>2</v>
       </c>
       <c r="J230" t="s">
-        <v>796</v>
+        <v>801</v>
       </c>
     </row>
     <row r="231" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>806</v>
+        <v>811</v>
       </c>
       <c r="B231" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C231" t="s">
-        <v>807</v>
+        <v>812</v>
       </c>
       <c r="D231" t="s">
         <v>20</v>
@@ -10084,18 +10069,18 @@
         <v>2</v>
       </c>
       <c r="J231" t="s">
-        <v>796</v>
+        <v>801</v>
       </c>
     </row>
     <row r="232" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>808</v>
+        <v>813</v>
       </c>
       <c r="B232" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C232" t="s">
-        <v>809</v>
+        <v>814</v>
       </c>
       <c r="D232" t="s">
         <v>20</v>
@@ -10104,18 +10089,18 @@
         <v>2</v>
       </c>
       <c r="J232" t="s">
-        <v>810</v>
+        <v>815</v>
       </c>
     </row>
     <row r="233" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>811</v>
+        <v>816</v>
       </c>
       <c r="B233" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C233" t="s">
-        <v>812</v>
+        <v>817</v>
       </c>
       <c r="D233" t="s">
         <v>20</v>
@@ -10127,7 +10112,7 @@
         <v>36</v>
       </c>
       <c r="G233" t="s">
-        <v>813</v>
+        <v>818</v>
       </c>
       <c r="H233" t="s">
         <v>27</v>
@@ -10135,13 +10120,13 @@
     </row>
     <row r="234" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>814</v>
+        <v>819</v>
       </c>
       <c r="B234" t="s">
-        <v>815</v>
+        <v>820</v>
       </c>
       <c r="C234" t="s">
-        <v>816</v>
+        <v>821</v>
       </c>
       <c r="D234" t="s">
         <v>20</v>
@@ -10153,21 +10138,21 @@
         <v>14</v>
       </c>
       <c r="G234" t="s">
-        <v>817</v>
+        <v>822</v>
       </c>
       <c r="H234" t="s">
-        <v>818</v>
+        <v>823</v>
       </c>
     </row>
     <row r="235" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>819</v>
+        <v>824</v>
       </c>
       <c r="B235" t="s">
-        <v>815</v>
+        <v>820</v>
       </c>
       <c r="C235" t="s">
-        <v>820</v>
+        <v>825</v>
       </c>
       <c r="D235" t="s">
         <v>20</v>
@@ -10179,24 +10164,24 @@
         <v>14</v>
       </c>
       <c r="G235" t="s">
-        <v>817</v>
+        <v>822</v>
       </c>
       <c r="H235" t="s">
-        <v>818</v>
+        <v>823</v>
       </c>
       <c r="J235" t="s">
-        <v>821</v>
+        <v>826</v>
       </c>
     </row>
     <row r="236" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>822</v>
+        <v>827</v>
       </c>
       <c r="B236" t="s">
-        <v>815</v>
+        <v>820</v>
       </c>
       <c r="C236" t="s">
-        <v>823</v>
+        <v>828</v>
       </c>
       <c r="D236" t="s">
         <v>20</v>
@@ -10211,18 +10196,18 @@
         <v>27</v>
       </c>
       <c r="J236" t="s">
-        <v>824</v>
+        <v>829</v>
       </c>
     </row>
     <row r="237" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>825</v>
+        <v>830</v>
       </c>
       <c r="B237" t="s">
-        <v>815</v>
+        <v>820</v>
       </c>
       <c r="C237" t="s">
-        <v>826</v>
+        <v>831</v>
       </c>
       <c r="D237" t="s">
         <v>20</v>
@@ -10234,27 +10219,27 @@
         <v>14</v>
       </c>
       <c r="G237" t="s">
-        <v>535</v>
+        <v>539</v>
       </c>
       <c r="H237" t="s">
-        <v>536</v>
+        <v>540</v>
       </c>
       <c r="I237" t="s">
-        <v>537</v>
+        <v>541</v>
       </c>
       <c r="J237" t="s">
-        <v>827</v>
+        <v>832</v>
       </c>
     </row>
     <row r="238" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>828</v>
+        <v>833</v>
       </c>
       <c r="B238" t="s">
-        <v>815</v>
+        <v>820</v>
       </c>
       <c r="C238" t="s">
-        <v>829</v>
+        <v>834</v>
       </c>
       <c r="D238" t="s">
         <v>20</v>
@@ -10266,27 +10251,27 @@
         <v>14</v>
       </c>
       <c r="G238" t="s">
-        <v>535</v>
+        <v>539</v>
       </c>
       <c r="H238" t="s">
-        <v>536</v>
+        <v>540</v>
       </c>
       <c r="I238" t="s">
-        <v>537</v>
+        <v>541</v>
       </c>
       <c r="J238" t="s">
-        <v>827</v>
+        <v>832</v>
       </c>
     </row>
     <row r="239" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>830</v>
+        <v>835</v>
       </c>
       <c r="B239" t="s">
-        <v>815</v>
+        <v>820</v>
       </c>
       <c r="C239" t="s">
-        <v>831</v>
+        <v>836</v>
       </c>
       <c r="D239" t="s">
         <v>20</v>
@@ -10298,27 +10283,27 @@
         <v>14</v>
       </c>
       <c r="G239" t="s">
-        <v>832</v>
+        <v>837</v>
       </c>
       <c r="H239" t="s">
-        <v>833</v>
+        <v>838</v>
       </c>
       <c r="I239" t="s">
-        <v>834</v>
+        <v>839</v>
       </c>
       <c r="J239" t="s">
-        <v>835</v>
+        <v>840</v>
       </c>
     </row>
     <row r="240" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>836</v>
+        <v>841</v>
       </c>
       <c r="B240" t="s">
-        <v>815</v>
+        <v>820</v>
       </c>
       <c r="C240" t="s">
-        <v>837</v>
+        <v>842</v>
       </c>
       <c r="D240" t="s">
         <v>20</v>
@@ -10327,30 +10312,30 @@
         <v>4</v>
       </c>
       <c r="F240" t="s">
-        <v>838</v>
+        <v>843</v>
       </c>
       <c r="G240" t="s">
-        <v>839</v>
+        <v>844</v>
       </c>
       <c r="H240" t="s">
-        <v>838</v>
+        <v>843</v>
       </c>
       <c r="I240">
         <v>570</v>
       </c>
       <c r="J240" t="s">
-        <v>840</v>
+        <v>845</v>
       </c>
     </row>
     <row r="241" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>841</v>
+        <v>846</v>
       </c>
       <c r="B241" t="s">
-        <v>815</v>
+        <v>820</v>
       </c>
       <c r="C241" t="s">
-        <v>842</v>
+        <v>847</v>
       </c>
       <c r="D241" t="s">
         <v>20</v>
@@ -10362,10 +10347,10 @@
         <v>14</v>
       </c>
       <c r="G241" t="s">
-        <v>843</v>
+        <v>848</v>
       </c>
       <c r="H241" t="s">
-        <v>844</v>
+        <v>849</v>
       </c>
       <c r="I241">
         <v>301652346813</v>
@@ -10373,13 +10358,13 @@
     </row>
     <row r="242" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>845</v>
+        <v>850</v>
       </c>
       <c r="B242" t="s">
-        <v>815</v>
+        <v>820</v>
       </c>
       <c r="C242" t="s">
-        <v>846</v>
+        <v>851</v>
       </c>
       <c r="D242" t="s">
         <v>49</v>
@@ -10391,7 +10376,7 @@
         <v>14</v>
       </c>
       <c r="G242" t="s">
-        <v>847</v>
+        <v>852</v>
       </c>
       <c r="H242" t="s">
         <v>27</v>
@@ -10399,13 +10384,13 @@
     </row>
     <row r="243" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>848</v>
+        <v>853</v>
       </c>
       <c r="B243" t="s">
-        <v>815</v>
+        <v>820</v>
       </c>
       <c r="C243" t="s">
-        <v>849</v>
+        <v>854</v>
       </c>
       <c r="D243" t="s">
         <v>20</v>
@@ -10417,7 +10402,7 @@
         <v>14</v>
       </c>
       <c r="G243" t="s">
-        <v>850</v>
+        <v>855</v>
       </c>
       <c r="H243" t="s">
         <v>27</v>
@@ -10425,13 +10410,13 @@
     </row>
     <row r="244" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>851</v>
+        <v>856</v>
       </c>
       <c r="B244" t="s">
-        <v>815</v>
+        <v>820</v>
       </c>
       <c r="C244" t="s">
-        <v>852</v>
+        <v>857</v>
       </c>
       <c r="D244" t="s">
         <v>49</v>
@@ -10443,24 +10428,24 @@
         <v>14</v>
       </c>
       <c r="G244" t="s">
-        <v>853</v>
+        <v>858</v>
       </c>
       <c r="H244" t="s">
         <v>27</v>
       </c>
       <c r="J244" t="s">
-        <v>854</v>
+        <v>859</v>
       </c>
     </row>
     <row r="245" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>855</v>
+        <v>860</v>
       </c>
       <c r="B245" t="s">
-        <v>815</v>
+        <v>820</v>
       </c>
       <c r="C245" t="s">
-        <v>856</v>
+        <v>861</v>
       </c>
       <c r="D245" t="s">
         <v>20</v>
@@ -10472,24 +10457,24 @@
         <v>14</v>
       </c>
       <c r="G245" t="s">
-        <v>857</v>
+        <v>862</v>
       </c>
       <c r="H245" t="s">
         <v>27</v>
       </c>
       <c r="J245" t="s">
-        <v>858</v>
+        <v>863</v>
       </c>
     </row>
     <row r="246" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>859</v>
+        <v>864</v>
       </c>
       <c r="B246" t="s">
-        <v>815</v>
+        <v>820</v>
       </c>
       <c r="C246" t="s">
-        <v>860</v>
+        <v>865</v>
       </c>
       <c r="D246" t="s">
         <v>20</v>
@@ -10501,24 +10486,24 @@
         <v>14</v>
       </c>
       <c r="G246" t="s">
-        <v>861</v>
+        <v>866</v>
       </c>
       <c r="H246" t="s">
         <v>27</v>
       </c>
       <c r="J246" t="s">
-        <v>862</v>
+        <v>867</v>
       </c>
     </row>
     <row r="247" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>863</v>
+        <v>868</v>
       </c>
       <c r="B247" t="s">
-        <v>815</v>
+        <v>820</v>
       </c>
       <c r="C247" t="s">
-        <v>864</v>
+        <v>869</v>
       </c>
       <c r="D247" t="s">
         <v>20</v>
@@ -10530,27 +10515,27 @@
         <v>14</v>
       </c>
       <c r="G247" t="s">
-        <v>865</v>
+        <v>870</v>
       </c>
       <c r="H247" t="s">
-        <v>866</v>
+        <v>871</v>
       </c>
       <c r="I247" t="s">
-        <v>867</v>
+        <v>872</v>
       </c>
       <c r="J247" t="s">
-        <v>868</v>
+        <v>873</v>
       </c>
     </row>
     <row r="248" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>869</v>
+        <v>874</v>
       </c>
       <c r="B248" t="s">
-        <v>815</v>
+        <v>820</v>
       </c>
       <c r="C248" t="s">
-        <v>870</v>
+        <v>875</v>
       </c>
       <c r="D248" t="s">
         <v>20</v>
@@ -10562,24 +10547,24 @@
         <v>14</v>
       </c>
       <c r="G248" t="s">
-        <v>871</v>
+        <v>876</v>
       </c>
       <c r="H248" t="s">
         <v>27</v>
       </c>
       <c r="J248" t="s">
-        <v>872</v>
+        <v>877</v>
       </c>
     </row>
     <row r="249" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>873</v>
+        <v>878</v>
       </c>
       <c r="B249" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="C249" t="s">
-        <v>875</v>
+        <v>880</v>
       </c>
       <c r="D249" t="s">
         <v>20</v>
@@ -10588,30 +10573,30 @@
         <v>2</v>
       </c>
       <c r="F249" t="s">
-        <v>876</v>
+        <v>881</v>
       </c>
       <c r="G249" t="s">
-        <v>877</v>
+        <v>882</v>
       </c>
       <c r="H249" t="s">
-        <v>878</v>
+        <v>883</v>
       </c>
       <c r="I249" t="s">
-        <v>879</v>
+        <v>884</v>
       </c>
       <c r="J249" t="s">
-        <v>880</v>
+        <v>885</v>
       </c>
     </row>
     <row r="250" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>881</v>
+        <v>886</v>
       </c>
       <c r="B250" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="C250" t="s">
-        <v>882</v>
+        <v>887</v>
       </c>
       <c r="D250" t="s">
         <v>20</v>
@@ -10620,30 +10605,30 @@
         <v>2</v>
       </c>
       <c r="F250" t="s">
-        <v>876</v>
+        <v>881</v>
       </c>
       <c r="G250" t="s">
+        <v>888</v>
+      </c>
+      <c r="H250" t="s">
         <v>883</v>
       </c>
-      <c r="H250" t="s">
-        <v>878</v>
-      </c>
       <c r="I250" t="s">
-        <v>884</v>
+        <v>889</v>
       </c>
       <c r="J250" t="s">
-        <v>885</v>
+        <v>890</v>
       </c>
     </row>
     <row r="251" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>886</v>
+        <v>891</v>
       </c>
       <c r="B251" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="C251" t="s">
-        <v>887</v>
+        <v>892</v>
       </c>
       <c r="D251" t="s">
         <v>20</v>
@@ -10652,27 +10637,27 @@
         <v>1</v>
       </c>
       <c r="F251" t="s">
-        <v>876</v>
+        <v>881</v>
       </c>
       <c r="G251" t="s">
-        <v>888</v>
+        <v>893</v>
       </c>
       <c r="H251" t="s">
-        <v>878</v>
+        <v>883</v>
       </c>
       <c r="I251" t="s">
-        <v>889</v>
+        <v>894</v>
       </c>
     </row>
     <row r="252" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>890</v>
+        <v>895</v>
       </c>
       <c r="B252" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="C252" t="s">
-        <v>891</v>
+        <v>896</v>
       </c>
       <c r="D252" t="s">
         <v>20</v>
@@ -10684,27 +10669,27 @@
         <v>14</v>
       </c>
       <c r="G252" t="s">
-        <v>892</v>
+        <v>897</v>
       </c>
       <c r="H252" t="s">
-        <v>833</v>
+        <v>838</v>
       </c>
       <c r="I252" t="s">
-        <v>893</v>
+        <v>898</v>
       </c>
       <c r="J252" t="s">
-        <v>894</v>
+        <v>899</v>
       </c>
     </row>
     <row r="253" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>895</v>
+        <v>900</v>
       </c>
       <c r="B253" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="C253" t="s">
-        <v>896</v>
+        <v>901</v>
       </c>
       <c r="D253" t="s">
         <v>20</v>
@@ -10716,27 +10701,27 @@
         <v>78</v>
       </c>
       <c r="G253" t="s">
-        <v>897</v>
+        <v>902</v>
       </c>
       <c r="H253" t="s">
-        <v>898</v>
+        <v>903</v>
       </c>
       <c r="I253" t="s">
-        <v>899</v>
+        <v>904</v>
       </c>
       <c r="J253" t="s">
-        <v>900</v>
+        <v>905</v>
       </c>
     </row>
     <row r="254" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>901</v>
+        <v>906</v>
       </c>
       <c r="B254" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="C254" t="s">
-        <v>902</v>
+        <v>907</v>
       </c>
       <c r="D254" t="s">
         <v>20</v>
@@ -10748,24 +10733,24 @@
         <v>78</v>
       </c>
       <c r="G254" t="s">
-        <v>903</v>
+        <v>908</v>
       </c>
       <c r="H254" t="s">
-        <v>904</v>
+        <v>909</v>
       </c>
       <c r="I254" t="s">
-        <v>905</v>
+        <v>910</v>
       </c>
     </row>
     <row r="255" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>906</v>
+        <v>911</v>
       </c>
       <c r="B255" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="C255" t="s">
-        <v>907</v>
+        <v>912</v>
       </c>
       <c r="D255" t="s">
         <v>20</v>
@@ -10777,24 +10762,24 @@
         <v>78</v>
       </c>
       <c r="G255" t="s">
-        <v>908</v>
+        <v>913</v>
       </c>
       <c r="H255" t="s">
-        <v>909</v>
+        <v>914</v>
       </c>
       <c r="I255" t="s">
-        <v>910</v>
+        <v>915</v>
       </c>
     </row>
     <row r="256" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>911</v>
+        <v>916</v>
       </c>
       <c r="B256" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="C256" t="s">
-        <v>912</v>
+        <v>917</v>
       </c>
       <c r="D256" t="s">
         <v>20</v>
@@ -10806,24 +10791,24 @@
         <v>14</v>
       </c>
       <c r="G256" t="s">
-        <v>913</v>
+        <v>918</v>
       </c>
       <c r="H256" t="s">
-        <v>914</v>
+        <v>919</v>
       </c>
       <c r="I256" t="s">
-        <v>915</v>
+        <v>920</v>
       </c>
     </row>
     <row r="257" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>916</v>
+        <v>921</v>
       </c>
       <c r="B257" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="C257" t="s">
-        <v>917</v>
+        <v>922</v>
       </c>
       <c r="D257" t="s">
         <v>20</v>
@@ -10835,7 +10820,7 @@
         <v>14</v>
       </c>
       <c r="G257" t="s">
-        <v>918</v>
+        <v>923</v>
       </c>
       <c r="H257" t="s">
         <v>27</v>
@@ -10843,13 +10828,13 @@
     </row>
     <row r="258" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>919</v>
+        <v>924</v>
       </c>
       <c r="B258" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="C258" t="s">
-        <v>920</v>
+        <v>925</v>
       </c>
       <c r="D258" t="s">
         <v>20</v>
@@ -10861,24 +10846,24 @@
         <v>14</v>
       </c>
       <c r="G258" t="s">
-        <v>921</v>
+        <v>926</v>
       </c>
       <c r="H258" t="s">
-        <v>922</v>
+        <v>927</v>
       </c>
       <c r="I258" t="s">
-        <v>923</v>
+        <v>928</v>
       </c>
     </row>
     <row r="259" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>924</v>
+        <v>929</v>
       </c>
       <c r="B259" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="C259" t="s">
-        <v>925</v>
+        <v>930</v>
       </c>
       <c r="D259" t="s">
         <v>20</v>
@@ -10890,24 +10875,24 @@
         <v>14</v>
       </c>
       <c r="G259" t="s">
-        <v>926</v>
+        <v>931</v>
       </c>
       <c r="H259" t="s">
-        <v>927</v>
+        <v>932</v>
       </c>
       <c r="J259" t="s">
-        <v>928</v>
+        <v>933</v>
       </c>
     </row>
     <row r="260" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>929</v>
+        <v>934</v>
       </c>
       <c r="B260" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="C260" t="s">
-        <v>930</v>
+        <v>935</v>
       </c>
       <c r="D260" t="s">
         <v>20</v>
@@ -10919,7 +10904,7 @@
         <v>14</v>
       </c>
       <c r="G260" t="s">
-        <v>931</v>
+        <v>936</v>
       </c>
       <c r="H260" t="s">
         <v>27</v>
@@ -10927,13 +10912,13 @@
     </row>
     <row r="261" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>932</v>
+        <v>937</v>
       </c>
       <c r="B261" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="C261" t="s">
-        <v>933</v>
+        <v>938</v>
       </c>
       <c r="D261" t="s">
         <v>20</v>
@@ -10945,7 +10930,7 @@
         <v>14</v>
       </c>
       <c r="G261" t="s">
-        <v>934</v>
+        <v>939</v>
       </c>
       <c r="H261" t="s">
         <v>27</v>
@@ -10953,13 +10938,13 @@
     </row>
     <row r="262" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>935</v>
+        <v>940</v>
       </c>
       <c r="B262" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="C262" t="s">
-        <v>936</v>
+        <v>941</v>
       </c>
       <c r="D262" t="s">
         <v>20</v>
@@ -10971,24 +10956,24 @@
         <v>14</v>
       </c>
       <c r="G262" t="s">
-        <v>937</v>
+        <v>942</v>
       </c>
       <c r="H262" t="s">
         <v>27</v>
       </c>
       <c r="J262" t="s">
-        <v>938</v>
+        <v>943</v>
       </c>
     </row>
     <row r="263" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>939</v>
+        <v>944</v>
       </c>
       <c r="B263" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="C263" t="s">
-        <v>940</v>
+        <v>945</v>
       </c>
       <c r="D263" t="s">
         <v>20</v>
@@ -11000,27 +10985,27 @@
         <v>14</v>
       </c>
       <c r="G263" t="s">
-        <v>941</v>
+        <v>946</v>
       </c>
       <c r="H263" t="s">
-        <v>942</v>
+        <v>947</v>
       </c>
       <c r="I263" t="s">
-        <v>943</v>
+        <v>948</v>
       </c>
       <c r="J263" t="s">
-        <v>944</v>
+        <v>949</v>
       </c>
     </row>
     <row r="264" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>945</v>
+        <v>950</v>
       </c>
       <c r="B264" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="C264" t="s">
-        <v>946</v>
+        <v>951</v>
       </c>
       <c r="D264" t="s">
         <v>20</v>
@@ -11032,27 +11017,27 @@
         <v>112</v>
       </c>
       <c r="G264" t="s">
-        <v>947</v>
+        <v>952</v>
       </c>
       <c r="H264" t="s">
         <v>508</v>
       </c>
       <c r="I264" t="s">
-        <v>948</v>
+        <v>953</v>
       </c>
       <c r="J264" t="s">
-        <v>949</v>
+        <v>954</v>
       </c>
     </row>
     <row r="265" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>950</v>
+        <v>955</v>
       </c>
       <c r="B265" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="C265" t="s">
-        <v>951</v>
+        <v>956</v>
       </c>
       <c r="D265" t="s">
         <v>20</v>
@@ -11064,24 +11049,24 @@
         <v>14</v>
       </c>
       <c r="G265" t="s">
-        <v>952</v>
+        <v>957</v>
       </c>
       <c r="H265" t="s">
         <v>27</v>
       </c>
       <c r="J265" t="s">
-        <v>953</v>
+        <v>958</v>
       </c>
     </row>
     <row r="266" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>954</v>
+        <v>959</v>
       </c>
       <c r="B266" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="C266" t="s">
-        <v>955</v>
+        <v>960</v>
       </c>
       <c r="D266" t="s">
         <v>20</v>
@@ -11093,7 +11078,7 @@
         <v>14</v>
       </c>
       <c r="G266" t="s">
-        <v>956</v>
+        <v>961</v>
       </c>
       <c r="H266" t="s">
         <v>27</v>
@@ -11101,13 +11086,13 @@
     </row>
     <row r="267" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>957</v>
+        <v>962</v>
       </c>
       <c r="B267" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="C267" t="s">
-        <v>958</v>
+        <v>963</v>
       </c>
       <c r="D267" t="s">
         <v>20</v>
@@ -11119,7 +11104,7 @@
         <v>14</v>
       </c>
       <c r="G267" t="s">
-        <v>959</v>
+        <v>964</v>
       </c>
       <c r="H267" t="s">
         <v>27</v>
@@ -11127,13 +11112,13 @@
     </row>
     <row r="268" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>960</v>
+        <v>965</v>
       </c>
       <c r="B268" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="C268" t="s">
-        <v>961</v>
+        <v>966</v>
       </c>
       <c r="D268" t="s">
         <v>25</v>
@@ -11145,7 +11130,7 @@
         <v>14</v>
       </c>
       <c r="G268" t="s">
-        <v>962</v>
+        <v>967</v>
       </c>
       <c r="H268" t="s">
         <v>27</v>
@@ -11153,13 +11138,13 @@
     </row>
     <row r="269" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>963</v>
+        <v>968</v>
       </c>
       <c r="B269" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="C269" t="s">
-        <v>964</v>
+        <v>969</v>
       </c>
       <c r="D269" t="s">
         <v>20</v>
@@ -11171,24 +11156,24 @@
         <v>14</v>
       </c>
       <c r="G269" t="s">
-        <v>965</v>
+        <v>970</v>
       </c>
       <c r="H269" t="s">
         <v>27</v>
       </c>
       <c r="J269" t="s">
-        <v>966</v>
+        <v>971</v>
       </c>
     </row>
     <row r="270" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>967</v>
+        <v>972</v>
       </c>
       <c r="B270" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="C270" t="s">
-        <v>968</v>
+        <v>973</v>
       </c>
       <c r="D270" t="s">
         <v>20</v>
@@ -11200,7 +11185,7 @@
         <v>14</v>
       </c>
       <c r="G270" t="s">
-        <v>969</v>
+        <v>974</v>
       </c>
       <c r="H270" t="s">
         <v>27</v>
@@ -11208,13 +11193,13 @@
     </row>
     <row r="271" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>970</v>
+        <v>975</v>
       </c>
       <c r="B271" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="C271" t="s">
-        <v>971</v>
+        <v>976</v>
       </c>
       <c r="D271" t="s">
         <v>20</v>
@@ -11226,24 +11211,24 @@
         <v>14</v>
       </c>
       <c r="G271" t="s">
-        <v>969</v>
+        <v>974</v>
       </c>
       <c r="H271" t="s">
-        <v>628</v>
+        <v>633</v>
       </c>
       <c r="I271" t="s">
-        <v>972</v>
+        <v>977</v>
       </c>
     </row>
     <row r="272" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>973</v>
+        <v>978</v>
       </c>
       <c r="B272" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="C272" t="s">
-        <v>974</v>
+        <v>979</v>
       </c>
       <c r="D272" t="s">
         <v>20</v>
@@ -11255,24 +11240,24 @@
         <v>14</v>
       </c>
       <c r="G272" t="s">
-        <v>975</v>
+        <v>980</v>
       </c>
       <c r="H272" t="s">
-        <v>818</v>
+        <v>823</v>
       </c>
       <c r="I272" t="s">
-        <v>976</v>
+        <v>981</v>
       </c>
     </row>
     <row r="273" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>977</v>
+        <v>982</v>
       </c>
       <c r="B273" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="C273" t="s">
-        <v>978</v>
+        <v>983</v>
       </c>
       <c r="D273" t="s">
         <v>20</v>
@@ -11284,24 +11269,24 @@
         <v>14</v>
       </c>
       <c r="G273" t="s">
-        <v>979</v>
+        <v>984</v>
       </c>
       <c r="H273" t="s">
-        <v>818</v>
+        <v>823</v>
       </c>
       <c r="I273" t="s">
-        <v>980</v>
+        <v>985</v>
       </c>
     </row>
     <row r="274" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>981</v>
+        <v>986</v>
       </c>
       <c r="B274" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="C274" t="s">
-        <v>982</v>
+        <v>987</v>
       </c>
       <c r="D274" t="s">
         <v>20</v>
@@ -11313,24 +11298,24 @@
         <v>14</v>
       </c>
       <c r="G274" t="s">
-        <v>983</v>
+        <v>988</v>
       </c>
       <c r="H274" t="s">
-        <v>818</v>
+        <v>823</v>
       </c>
       <c r="I274" t="s">
-        <v>984</v>
+        <v>989</v>
       </c>
     </row>
     <row r="275" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>985</v>
+        <v>990</v>
       </c>
       <c r="B275" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="C275" t="s">
-        <v>986</v>
+        <v>991</v>
       </c>
       <c r="D275" t="s">
         <v>20</v>
@@ -11342,24 +11327,24 @@
         <v>78</v>
       </c>
       <c r="G275" t="s">
-        <v>987</v>
+        <v>992</v>
       </c>
       <c r="H275" t="s">
-        <v>988</v>
+        <v>993</v>
       </c>
       <c r="I275" t="s">
-        <v>989</v>
+        <v>994</v>
       </c>
     </row>
     <row r="276" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>990</v>
+        <v>995</v>
       </c>
       <c r="B276" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="C276" t="s">
-        <v>991</v>
+        <v>996</v>
       </c>
       <c r="D276" t="s">
         <v>20</v>
@@ -11371,24 +11356,24 @@
         <v>14</v>
       </c>
       <c r="G276" t="s">
-        <v>992</v>
+        <v>997</v>
       </c>
       <c r="H276" t="s">
-        <v>993</v>
+        <v>998</v>
       </c>
       <c r="I276" t="s">
-        <v>994</v>
+        <v>999</v>
       </c>
     </row>
     <row r="277" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>995</v>
+        <v>1000</v>
       </c>
       <c r="B277" t="s">
-        <v>996</v>
+        <v>1001</v>
       </c>
       <c r="C277" t="s">
-        <v>997</v>
+        <v>1002</v>
       </c>
       <c r="D277" t="s">
         <v>20</v>
@@ -11400,10 +11385,10 @@
         <v>14</v>
       </c>
       <c r="G277" t="s">
-        <v>998</v>
+        <v>1003</v>
       </c>
       <c r="H277" t="s">
-        <v>999</v>
+        <v>1004</v>
       </c>
       <c r="I277">
         <v>92003</v>
@@ -11411,13 +11396,13 @@
     </row>
     <row r="278" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>1000</v>
+        <v>1005</v>
       </c>
       <c r="B278" t="s">
-        <v>996</v>
+        <v>1001</v>
       </c>
       <c r="C278" t="s">
-        <v>1001</v>
+        <v>1006</v>
       </c>
       <c r="D278" t="s">
         <v>20</v>
@@ -11432,18 +11417,18 @@
         <v>27</v>
       </c>
       <c r="J278" t="s">
-        <v>1002</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="279" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>1003</v>
+        <v>1008</v>
       </c>
       <c r="B279" t="s">
-        <v>996</v>
+        <v>1001</v>
       </c>
       <c r="C279" t="s">
-        <v>1004</v>
+        <v>1009</v>
       </c>
       <c r="D279" t="s">
         <v>25</v>
@@ -11455,7 +11440,7 @@
         <v>14</v>
       </c>
       <c r="G279" t="s">
-        <v>1005</v>
+        <v>1010</v>
       </c>
       <c r="H279" t="s">
         <v>27</v>
@@ -11463,13 +11448,13 @@
     </row>
     <row r="280" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>1006</v>
+        <v>1011</v>
       </c>
       <c r="B280" t="s">
-        <v>996</v>
+        <v>1001</v>
       </c>
       <c r="C280" t="s">
-        <v>1007</v>
+        <v>1012</v>
       </c>
       <c r="D280" t="s">
         <v>20</v>
@@ -11481,7 +11466,7 @@
         <v>14</v>
       </c>
       <c r="G280" t="s">
-        <v>1008</v>
+        <v>1013</v>
       </c>
       <c r="H280" t="s">
         <v>27</v>
@@ -11489,13 +11474,13 @@
     </row>
     <row r="281" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>1009</v>
+        <v>1014</v>
       </c>
       <c r="B281" t="s">
-        <v>996</v>
+        <v>1001</v>
       </c>
       <c r="C281" t="s">
-        <v>1010</v>
+        <v>1015</v>
       </c>
       <c r="D281" t="s">
         <v>20</v>
@@ -11507,18 +11492,18 @@
         <v>27</v>
       </c>
       <c r="J281" t="s">
-        <v>1011</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="282" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>1012</v>
+        <v>1017</v>
       </c>
       <c r="B282" t="s">
-        <v>996</v>
+        <v>1001</v>
       </c>
       <c r="C282" t="s">
-        <v>1013</v>
+        <v>1018</v>
       </c>
       <c r="D282" t="s">
         <v>20</v>
@@ -11532,13 +11517,13 @@
     </row>
     <row r="283" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>1014</v>
+        <v>1019</v>
       </c>
       <c r="B283" t="s">
-        <v>996</v>
+        <v>1001</v>
       </c>
       <c r="C283" t="s">
-        <v>1015</v>
+        <v>1020</v>
       </c>
       <c r="D283" t="s">
         <v>20</v>
@@ -11550,24 +11535,24 @@
         <v>14</v>
       </c>
       <c r="G283" t="s">
-        <v>1016</v>
+        <v>1021</v>
       </c>
       <c r="H283" t="s">
         <v>27</v>
       </c>
       <c r="J283" t="s">
-        <v>1017</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="284" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>1018</v>
+        <v>1023</v>
       </c>
       <c r="B284" t="s">
-        <v>996</v>
+        <v>1001</v>
       </c>
       <c r="C284" t="s">
-        <v>1019</v>
+        <v>1024</v>
       </c>
       <c r="D284" t="s">
         <v>20</v>
@@ -11578,13 +11563,13 @@
     </row>
     <row r="285" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>1020</v>
+        <v>1025</v>
       </c>
       <c r="B285" t="s">
-        <v>996</v>
+        <v>1001</v>
       </c>
       <c r="C285" t="s">
-        <v>1021</v>
+        <v>1026</v>
       </c>
       <c r="D285" t="s">
         <v>20</v>
@@ -11596,10 +11581,10 @@
         <v>14</v>
       </c>
       <c r="G285" t="s">
-        <v>1022</v>
+        <v>1027</v>
       </c>
       <c r="H285" t="s">
-        <v>1023</v>
+        <v>1028</v>
       </c>
       <c r="I285">
         <v>2078216</v>
@@ -11607,13 +11592,13 @@
     </row>
     <row r="286" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>1024</v>
+        <v>1029</v>
       </c>
       <c r="B286" t="s">
-        <v>996</v>
+        <v>1001</v>
       </c>
       <c r="C286" t="s">
-        <v>1025</v>
+        <v>1030</v>
       </c>
       <c r="D286" t="s">
         <v>20</v>
@@ -11624,13 +11609,13 @@
     </row>
     <row r="287" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>1026</v>
+        <v>1031</v>
       </c>
       <c r="B287" t="s">
-        <v>996</v>
+        <v>1001</v>
       </c>
       <c r="C287" t="s">
-        <v>1027</v>
+        <v>1032</v>
       </c>
       <c r="D287" t="s">
         <v>20</v>
@@ -11642,24 +11627,24 @@
         <v>14</v>
       </c>
       <c r="G287" t="s">
-        <v>1028</v>
+        <v>1033</v>
       </c>
       <c r="H287" t="s">
-        <v>1029</v>
+        <v>1034</v>
       </c>
       <c r="I287" t="s">
-        <v>1030</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="288" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>1031</v>
+        <v>1036</v>
       </c>
       <c r="B288" t="s">
-        <v>996</v>
+        <v>1001</v>
       </c>
       <c r="C288" t="s">
-        <v>1032</v>
+        <v>1037</v>
       </c>
       <c r="D288" t="s">
         <v>20</v>
@@ -11668,18 +11653,18 @@
         <v>1</v>
       </c>
       <c r="J288" t="s">
-        <v>1033</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="289" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>1034</v>
+        <v>1039</v>
       </c>
       <c r="B289" t="s">
-        <v>996</v>
+        <v>1001</v>
       </c>
       <c r="C289" t="s">
-        <v>1035</v>
+        <v>1040</v>
       </c>
       <c r="D289" t="s">
         <v>20</v>
@@ -11691,27 +11676,27 @@
         <v>14</v>
       </c>
       <c r="G289" t="s">
-        <v>1036</v>
+        <v>1041</v>
       </c>
       <c r="H289" t="s">
-        <v>1037</v>
+        <v>1042</v>
       </c>
       <c r="I289" t="s">
-        <v>1038</v>
+        <v>1043</v>
       </c>
       <c r="J289" t="s">
-        <v>1039</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="290" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>1040</v>
+        <v>1045</v>
       </c>
       <c r="B290" t="s">
-        <v>996</v>
+        <v>1001</v>
       </c>
       <c r="C290" t="s">
-        <v>1041</v>
+        <v>1046</v>
       </c>
       <c r="D290" t="s">
         <v>25</v>
@@ -11722,13 +11707,13 @@
     </row>
     <row r="291" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>1042</v>
+        <v>1047</v>
       </c>
       <c r="B291" t="s">
-        <v>996</v>
+        <v>1001</v>
       </c>
       <c r="C291" t="s">
-        <v>1043</v>
+        <v>1048</v>
       </c>
       <c r="D291" t="s">
         <v>20</v>
@@ -11743,18 +11728,18 @@
         <v>27</v>
       </c>
       <c r="J291" t="s">
-        <v>1044</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="292" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>1045</v>
+        <v>1050</v>
       </c>
       <c r="B292" t="s">
-        <v>996</v>
+        <v>1001</v>
       </c>
       <c r="C292" t="s">
-        <v>1046</v>
+        <v>1051</v>
       </c>
       <c r="D292" t="s">
         <v>25</v>
@@ -11763,14 +11748,13 @@
         <v>1</v>
       </c>
       <c r="J292" t="s">
-        <v>1047</v>
+        <v>1052</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>